<commit_message>
NAV-60 test data set that loads correctly
</commit_message>
<xml_diff>
--- a/navigator_engine/tests/test_data/Estimates Test Data.xlsx
+++ b/navigator_engine/tests/test_data/Estimates Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soppe\Documents\Projects\navigator_engine\navigator_engine\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103B96C3-442E-40E5-A46F-639C4BC0DD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69384F3A-00CC-4B49-AC48-D0676C5E0ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="00-Overview" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="177">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -867,22 +867,10 @@
     <t>check_manual_confirmation('EST-MCN-03-A')</t>
   </si>
   <si>
-    <t>check_manual_confirmation('EST-MCN-04-A')</t>
-  </si>
-  <si>
-    <t>check_manual_confirmation('EST-MCN-05-A')</t>
-  </si>
-  <si>
     <t>check_manual_confirmation('EST-MCN-06-A')</t>
   </si>
   <si>
     <t>check_manual_confirmation('EST-FOR-01-A')</t>
-  </si>
-  <si>
-    <t>check_manual_confirmation('EST-FOR-02-A')</t>
-  </si>
-  <si>
-    <t>check_manual_confirmation('EST-FOR-CK-02-A')</t>
   </si>
   <si>
     <t>check_manual_confirmation('EST-FOR-03-A')</t>
@@ -900,16 +888,16 @@
     <t>check_manual_confirmation('EST-LOP-02-A')</t>
   </si>
   <si>
-    <t>check_manual_confirmation('EST-LOP-CK-02-A')</t>
-  </si>
-  <si>
-    <t>check_manual_confirmation('EST-LOP-03-A')</t>
-  </si>
-  <si>
     <t>check_manual_confirmation('EST-LOP-04-A')</t>
   </si>
   <si>
     <t>check_manual_confirmation('EST-LOP-05-A')</t>
+  </si>
+  <si>
+    <t>return_true()</t>
+  </si>
+  <si>
+    <t>return_false()</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1338,9 +1326,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1573,8 +1558,8 @@
   <dimension ref="A1:AA993"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1596,14 +1581,14 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="75" t="s">
+      <c r="C1" s="75"/>
+      <c r="D1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="76"/>
+      <c r="E1" s="75"/>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1633,14 +1618,14 @@
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="77" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="76"/>
+      <c r="E2" s="75"/>
       <c r="F2" s="6">
         <v>0.1</v>
       </c>
@@ -30486,7 +30471,7 @@
   <dimension ref="A1:K996"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -30509,14 +30494,14 @@
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="79" t="s">
+      <c r="C1" s="75"/>
+      <c r="D1" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="76"/>
+      <c r="E1" s="75"/>
       <c r="F1" s="31" t="s">
         <v>3</v>
       </c>
@@ -30527,14 +30512,14 @@
       <c r="A2" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="80" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="76"/>
+      <c r="E2" s="75"/>
       <c r="F2" s="34">
         <v>0.1</v>
       </c>
@@ -32073,8 +32058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E6" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32095,10 +32080,10 @@
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76"/>
+      <c r="C1" s="75"/>
       <c r="D1" s="30" t="s">
         <v>2</v>
       </c>
@@ -32111,10 +32096,10 @@
       <c r="A2" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="76"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="33" t="s">
         <v>97</v>
       </c>
@@ -32257,8 +32242,8 @@
       <c r="J7" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="K7" s="19" t="s">
-        <v>166</v>
+      <c r="K7" s="27" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="102.6" x14ac:dyDescent="0.25">
@@ -32288,8 +32273,8 @@
       <c r="J8" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="K8" s="19" t="s">
-        <v>167</v>
+      <c r="K8" s="20" t="s">
+        <v>175</v>
       </c>
       <c r="M8" s="67"/>
       <c r="N8" s="67"/>
@@ -32332,7 +32317,7 @@
       <c r="I9" s="45"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -32355,8 +32340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K10"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32378,10 +32363,10 @@
       <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76"/>
+      <c r="C1" s="75"/>
       <c r="D1" s="30" t="s">
         <v>2</v>
       </c>
@@ -32394,14 +32379,14 @@
       <c r="A2" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="79" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="80" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="79" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="76"/>
+      <c r="E2" s="75"/>
       <c r="F2" s="34">
         <v>0.1</v>
       </c>
@@ -32475,7 +32460,7 @@
       </c>
       <c r="I5" s="27"/>
       <c r="J5" s="27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="82.2" x14ac:dyDescent="0.25">
@@ -32505,7 +32490,7 @@
         <v>150</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
@@ -32530,8 +32515,8 @@
       <c r="I7" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="J7" s="72" t="s">
-        <v>171</v>
+      <c r="J7" s="20" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
@@ -32559,7 +32544,7 @@
       <c r="H8" s="50"/>
       <c r="I8" s="27"/>
       <c r="J8" s="27" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
@@ -32587,7 +32572,7 @@
       <c r="H9" s="50"/>
       <c r="I9" s="25"/>
       <c r="J9" s="27" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="154.19999999999999" x14ac:dyDescent="0.3">
@@ -32611,9 +32596,9 @@
         <v>0</v>
       </c>
       <c r="H10" s="45"/>
-      <c r="I10" s="73"/>
+      <c r="I10" s="72"/>
       <c r="J10" s="27" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -33695,8 +33680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22721940-25D6-460C-A4BF-0F3B1609DF6D}">
   <dimension ref="A1:J1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -33718,10 +33703,10 @@
       <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76"/>
+      <c r="C1" s="75"/>
       <c r="D1" s="30" t="s">
         <v>2</v>
       </c>
@@ -33734,14 +33719,14 @@
       <c r="A2" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="79" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="80" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="79" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="76"/>
+      <c r="E2" s="75"/>
       <c r="F2" s="34">
         <v>0.1</v>
       </c>
@@ -33815,7 +33800,7 @@
       </c>
       <c r="I5" s="27"/>
       <c r="J5" s="27" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="82.2" x14ac:dyDescent="0.25">
@@ -33843,7 +33828,7 @@
       <c r="H6" s="50"/>
       <c r="I6" s="27"/>
       <c r="J6" s="27" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
@@ -33865,9 +33850,11 @@
       <c r="H7" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74" t="s">
-        <v>177</v>
+      <c r="I7" s="73" t="s">
+        <v>154</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
@@ -33897,7 +33884,7 @@
         <v>154</v>
       </c>
       <c r="J8" s="27" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
@@ -33925,7 +33912,7 @@
       <c r="H9" s="50"/>
       <c r="I9" s="25"/>
       <c r="J9" s="27" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="154.19999999999999" x14ac:dyDescent="0.3">
@@ -33949,9 +33936,9 @@
         <v>0</v>
       </c>
       <c r="H10" s="46"/>
-      <c r="I10" s="73"/>
+      <c r="I10" s="72"/>
       <c r="J10" s="27" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
NAV-60 avoid looping workflow that loops into beginning
</commit_message>
<xml_diff>
--- a/navigator_engine/tests/test_data/Estimates Test Data.xlsx
+++ b/navigator_engine/tests/test_data/Estimates Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soppe\Documents\Projects\navigator_engine\navigator_engine\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69384F3A-00CC-4B49-AC48-D0676C5E0ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB73688-5AA5-4046-926F-857BE025F827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="178">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -101,9 +101,6 @@
   </si>
   <si>
     <t>Complete Message</t>
-  </si>
-  <si>
-    <t>HIV Estimates Process 2022</t>
   </si>
   <si>
     <r>
@@ -232,9 +229,6 @@
   </si>
   <si>
     <t>Milestone: Enter Data Into Spectrum</t>
-  </si>
-  <si>
-    <t>Preparing Input Data for HIV Estimates</t>
   </si>
   <si>
     <r>
@@ -524,32 +518,6 @@
     <t>check_manual_confirmation('EST-GEN-09-A')</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">Upload Estimates Inputs Data </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF9900FF"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">Templates </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>to ADR</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Once you have prepared your data inputs, you can upload the files to your organization/country on the AIDS Data Repository (ADR). There are many advantages to using ADR, including integration with key estimates models such as ShinyRob and Naomi. Before you begin this step, you should be sure you have populated all required inputs templates (e.g., area boundary files, programme data, surveys). You will need to have an ADR user account and be associated with an organization (country) with an editor role. </t>
   </si>
   <si>
@@ -696,9 +664,6 @@
       </rPr>
       <t>https://adr.unaids.org/</t>
     </r>
-  </si>
-  <si>
-    <t>Review quality of programme data inputs in ShinyRob</t>
   </si>
   <si>
     <r>
@@ -898,6 +863,21 @@
   </si>
   <si>
     <t>return_false()</t>
+  </si>
+  <si>
+    <t>Simple Workflow</t>
+  </si>
+  <si>
+    <t>Test Data Overview</t>
+  </si>
+  <si>
+    <t>Multiple Complete Nodes</t>
+  </si>
+  <si>
+    <t>Forking Workflow</t>
+  </si>
+  <si>
+    <t>Looping workflow</t>
   </si>
 </sst>
 </file>
@@ -1559,7 +1539,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1616,21 +1596,21 @@
     </row>
     <row r="2" spans="1:27" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>5</v>
+        <v>174</v>
       </c>
       <c r="B2" s="76" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="75"/>
       <c r="D2" s="76" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="75"/>
       <c r="F2" s="6">
         <v>0.1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="8"/>
       <c r="K2" s="5"/>
@@ -1682,37 +1662,37 @@
     </row>
     <row r="4" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="G4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="H4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="I4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="J4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="L4" s="14" t="s">
         <v>18</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>19</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -1731,23 +1711,23 @@
     </row>
     <row r="5" spans="1:27" ht="123" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="D5" s="17" t="s">
         <v>22</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="18">
         <v>1</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
@@ -1770,23 +1750,23 @@
     </row>
     <row r="6" spans="1:27" ht="93" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="C6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="17" t="s">
         <v>27</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>28</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="18">
         <v>1</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
@@ -1809,13 +1789,13 @@
     </row>
     <row r="7" spans="1:27" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>31</v>
-      </c>
       <c r="C7" s="16" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
@@ -1844,13 +1824,13 @@
     </row>
     <row r="8" spans="1:27" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>33</v>
-      </c>
       <c r="C8" s="17" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -1879,13 +1859,13 @@
     </row>
     <row r="9" spans="1:27" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>35</v>
-      </c>
       <c r="C9" s="17" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
@@ -1914,13 +1894,13 @@
     </row>
     <row r="10" spans="1:27" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>37</v>
-      </c>
       <c r="C10" s="16" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -30472,7 +30452,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -30510,14 +30490,14 @@
     </row>
     <row r="2" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
-        <v>38</v>
+        <v>173</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="75"/>
       <c r="D2" s="79" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="75"/>
       <c r="F2" s="34">
@@ -30538,169 +30518,169 @@
     </row>
     <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="C4" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="D4" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="E4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="F4" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="G4" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="5" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="D5" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="E5" s="47" t="s">
         <v>42</v>
-      </c>
-      <c r="D5" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="47" t="s">
-        <v>44</v>
       </c>
       <c r="F5" s="48"/>
       <c r="G5" s="49">
         <v>0</v>
       </c>
       <c r="H5" s="45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I5" s="45"/>
       <c r="J5" s="19"/>
       <c r="K5" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="44" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="102.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="C6" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="D6" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="E6" s="47" t="s">
         <v>49</v>
-      </c>
-      <c r="D6" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="47" t="s">
-        <v>51</v>
       </c>
       <c r="F6" s="50"/>
       <c r="G6" s="51">
         <v>1</v>
       </c>
       <c r="H6" s="45" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I6" s="45"/>
       <c r="J6" s="19"/>
       <c r="K6" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="44" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="C7" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="D7" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="E7" s="46" t="s">
         <v>56</v>
-      </c>
-      <c r="D7" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>58</v>
       </c>
       <c r="F7" s="48"/>
       <c r="G7" s="49">
         <v>1</v>
       </c>
       <c r="H7" s="52" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I7" s="53" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="204.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="44" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="204.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="C8" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="D8" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="E8" s="46" t="s">
         <v>64</v>
-      </c>
-      <c r="D8" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="46" t="s">
-        <v>66</v>
       </c>
       <c r="F8" s="48"/>
       <c r="G8" s="49">
         <v>1</v>
       </c>
       <c r="H8" s="53" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I8" s="53"/>
       <c r="J8" s="19"/>
       <c r="K8" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="286.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="44" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="286.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="C9" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="D9" s="45" t="s">
         <v>70</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="45" t="s">
-        <v>72</v>
       </c>
       <c r="E9" s="45"/>
       <c r="F9" s="48">
@@ -30710,28 +30690,28 @@
         <v>1</v>
       </c>
       <c r="H9" s="53" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I9" s="53" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="61.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="44" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="61.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="C10" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="D10" s="45" t="s">
         <v>77</v>
-      </c>
-      <c r="C10" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>79</v>
       </c>
       <c r="E10" s="45"/>
       <c r="F10" s="48"/>
@@ -30739,28 +30719,28 @@
         <v>0</v>
       </c>
       <c r="H10" s="53" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I10" s="53" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J10" s="19"/>
       <c r="K10" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+      <c r="A11" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="44" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="C11" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="D11" s="45" t="s">
         <v>84</v>
-      </c>
-      <c r="C11" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="45" t="s">
-        <v>86</v>
       </c>
       <c r="E11" s="45"/>
       <c r="F11" s="48"/>
@@ -30768,28 +30748,28 @@
         <v>0</v>
       </c>
       <c r="H11" s="32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I11" s="54" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J11" s="19"/>
       <c r="K11" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="44" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="C12" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="D12" s="45" t="s">
         <v>91</v>
-      </c>
-      <c r="C12" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="45" t="s">
-        <v>93</v>
       </c>
       <c r="E12" s="45"/>
       <c r="F12" s="55"/>
@@ -30800,7 +30780,7 @@
       <c r="I12" s="32"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32059,7 +32039,7 @@
   <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32094,14 +32074,14 @@
     </row>
     <row r="2" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>95</v>
+        <v>175</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C2" s="75"/>
       <c r="D2" s="33" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E2" s="59"/>
       <c r="F2" s="34">
@@ -32120,54 +32100,54 @@
     </row>
     <row r="4" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="C4" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="D4" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="E4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="F4" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="G4" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="5" spans="1:26" ht="72" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F5" s="64">
         <v>1</v>
@@ -32176,26 +32156,26 @@
         <v>0</v>
       </c>
       <c r="H5" s="45" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I5" s="45"/>
       <c r="J5" s="19"/>
       <c r="K5" s="19" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A6" s="63" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E6" s="45"/>
       <c r="F6" s="65">
@@ -32205,29 +32185,29 @@
         <v>0</v>
       </c>
       <c r="H6" s="53" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I6" s="53"/>
       <c r="J6" s="19"/>
       <c r="K6" s="19" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="82.2" x14ac:dyDescent="0.25">
       <c r="A7" s="63" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B7" s="45" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D7" s="45" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F7" s="65">
         <v>0</v>
@@ -32236,28 +32216,28 @@
         <v>0</v>
       </c>
       <c r="H7" s="45" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I7" s="45"/>
       <c r="J7" s="19" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="K7" s="27" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="102.6" x14ac:dyDescent="0.25">
       <c r="A8" s="63" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E8" s="45"/>
       <c r="F8" s="65">
@@ -32267,14 +32247,14 @@
         <v>0</v>
       </c>
       <c r="H8" s="66" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I8" s="45"/>
       <c r="J8" s="19" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M8" s="67"/>
       <c r="N8" s="67"/>
@@ -32293,19 +32273,19 @@
     </row>
     <row r="9" spans="1:26" ht="72" x14ac:dyDescent="0.25">
       <c r="A9" s="63" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D9" s="45" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E9" s="47" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F9" s="46">
         <v>0</v>
@@ -32317,7 +32297,7 @@
       <c r="I9" s="45"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -32340,8 +32320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32377,14 +32357,14 @@
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>119</v>
+        <v>176</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C2" s="75"/>
       <c r="D2" s="79" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E2" s="75"/>
       <c r="F2" s="34">
@@ -32403,51 +32383,51 @@
     </row>
     <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="C4" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="D4" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="E4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="F4" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="G4" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="5" spans="1:10" ht="102.6" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F5" s="48">
         <v>1</v>
@@ -32456,28 +32436,28 @@
         <v>0</v>
       </c>
       <c r="H5" s="66" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I5" s="27"/>
       <c r="J5" s="27" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="82.2" x14ac:dyDescent="0.25">
       <c r="A6" s="45" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B6" s="45" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F6" s="48">
         <v>1</v>
@@ -32487,19 +32467,19 @@
       </c>
       <c r="H6" s="50"/>
       <c r="I6" s="46" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="69" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B7" s="69"/>
       <c r="C7" s="69" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D7" s="69"/>
       <c r="E7" s="69"/>
@@ -32510,30 +32490,30 @@
         <v>1</v>
       </c>
       <c r="H7" s="71" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I7" s="46" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F8" s="48">
         <v>1</v>
@@ -32544,24 +32524,24 @@
       <c r="H8" s="50"/>
       <c r="I8" s="27"/>
       <c r="J8" s="27" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D9" s="45" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F9" s="50">
         <v>1</v>
@@ -32572,21 +32552,21 @@
       <c r="H9" s="50"/>
       <c r="I9" s="25"/>
       <c r="J9" s="27" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="154.19999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="45" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B10" s="45" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E10" s="45"/>
       <c r="F10" s="48">
@@ -32598,7 +32578,7 @@
       <c r="H10" s="45"/>
       <c r="I10" s="72"/>
       <c r="J10" s="27" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -33680,8 +33660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22721940-25D6-460C-A4BF-0F3B1609DF6D}">
   <dimension ref="A1:J1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -33717,14 +33697,14 @@
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>119</v>
+        <v>177</v>
       </c>
       <c r="B2" s="79" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C2" s="75"/>
       <c r="D2" s="79" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E2" s="75"/>
       <c r="F2" s="34">
@@ -33743,51 +33723,51 @@
     </row>
     <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="C4" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="D4" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="E4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="F4" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="G4" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="5" spans="1:10" ht="102.6" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F5" s="48">
         <v>1</v>
@@ -33796,28 +33776,28 @@
         <v>0</v>
       </c>
       <c r="H5" s="66" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I5" s="27"/>
       <c r="J5" s="27" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="82.2" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F6" s="48">
         <v>1</v>
@@ -33828,16 +33808,16 @@
       <c r="H6" s="50"/>
       <c r="I6" s="27"/>
       <c r="J6" s="27" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="69" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B7" s="69"/>
       <c r="C7" s="69" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D7" s="69"/>
       <c r="E7" s="69"/>
@@ -33848,30 +33828,30 @@
         <v>1</v>
       </c>
       <c r="H7" s="71" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I7" s="73" t="s">
+        <v>149</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="J7" s="27" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
-        <v>158</v>
-      </c>
       <c r="B8" s="46" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F8" s="48">
         <v>1</v>
@@ -33881,27 +33861,27 @@
       </c>
       <c r="H8" s="50"/>
       <c r="I8" s="46" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="J8" s="27" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D9" s="46" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F9" s="50">
         <v>1</v>
@@ -33912,21 +33892,21 @@
       <c r="H9" s="50"/>
       <c r="I9" s="25"/>
       <c r="J9" s="27" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="154.19999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D10" s="46" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E10" s="46"/>
       <c r="F10" s="48">
@@ -33938,7 +33918,7 @@
       <c r="H10" s="46"/>
       <c r="I10" s="72"/>
       <c r="J10" s="27" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
NAV-254 update test data
</commit_message>
<xml_diff>
--- a/navigator_engine/tests/test_data/Estimates Test Data.xlsx
+++ b/navigator_engine/tests/test_data/Estimates Test Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soppe\Documents\Projects\navigator_engine\navigator_engine\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378F5DF2-92BB-409D-AD70-9363C83A7F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1754BC-FEF2-4AC9-92F0-31DBD39A467B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="00-Overview" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,18 @@
     <sheet name="03-ForkingWorkflow" sheetId="4" r:id="rId4"/>
     <sheet name="04-LoopingWorkflow" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -83,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="187">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -1212,9 +1222,6 @@
     <t>check_manual_confirmation('EST-GEN-07-01-A')</t>
   </si>
   <si>
-    <t>Test Data Overview FRENCH</t>
-  </si>
-  <si>
     <r>
       <t>In this milestone, you will prepare</t>
     </r>
@@ -1239,13 +1246,7 @@
     </r>
   </si>
   <si>
-    <t>In this milestone, you will prepare and place the required input data in the templates needed to generate HIV estimates. You should use the best, highest quality, and most complete input data you have available to you for the estimates process.  FRENCH</t>
-  </si>
-  <si>
     <t>FR::Complete Message</t>
-  </si>
-  <si>
-    <t>Congratulations, you have completed this year's estimates process. You may now use your results for other needs such as the PEPFAR data pack, DMPPT2 (for VMMC data where applicable), national reporting, or other needs. FRENCH</t>
   </si>
   <si>
     <t>FRENCH</t>
@@ -1273,7 +1274,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1374,6 +1375,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1493,7 +1500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1602,12 +1609,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1619,11 +1620,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2009,9 +2022,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD993"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2035,20 +2048,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C1" s="54" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
-        <v>185</v>
-      </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54" t="s">
+      <c r="D1" s="52"/>
+      <c r="E1" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="54"/>
+      <c r="H1" s="52"/>
       <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2056,7 +2069,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="51" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
@@ -2080,29 +2093,32 @@
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="61" t="str">
+        <f>_xlfn.CONCAT("FRENCH ", A2)</f>
+        <v>FRENCH Test Data Overview</v>
+      </c>
+      <c r="C2" s="62" t="s">
         <v>178</v>
       </c>
-      <c r="C2" s="55" t="s">
-        <v>179</v>
-      </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55" t="s">
-        <v>180</v>
-      </c>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55" t="s">
+      <c r="D2" s="53"/>
+      <c r="E2" s="53" t="str">
+        <f>_xlfn.CONCAT("FRENCH ", C2)</f>
+        <v xml:space="preserve">FRENCH In this milestone, you will prepare and place the required input data in the templates needed to generate HIV estimates. You should use the best, highest quality, and most complete input data you have available to you for the estimates process. </v>
+      </c>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="55"/>
+      <c r="H2" s="53"/>
       <c r="I2" s="5">
         <v>0.1</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>182</v>
+      <c r="K2" s="5" t="str">
+        <f>_xlfn.CONCAT("FRENCH ", J2)</f>
+        <v>FRENCH Congratulations, you have completed this year's estimates process. You may now use your results for other needs such as the PEPFAR data pack, DMPPT2 (for VMMC data where applicable), national reporting, or other needs.</v>
       </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -2151,7 +2167,7 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
     </row>
-    <row r="4" spans="1:30" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -2159,7 +2175,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>11</v>
@@ -2168,13 +2184,13 @@
         <v>12</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>14</v>
@@ -2209,15 +2225,16 @@
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
     </row>
-    <row r="5" spans="1:30" ht="286.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>183</v>
+      <c r="C5" s="61" t="str">
+        <f>_xlfn.CONCAT("FRENCH ", B5)</f>
+        <v>FRENCH Welcome to the Navigator</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>22</v>
@@ -2225,8 +2242,11 @@
       <c r="E5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>183</v>
+      <c r="F5" s="15" t="str">
+        <f>_xlfn.CONCAT("FRENCH ", E5)</f>
+        <v xml:space="preserve">FRENCH Welcome to the HIV Estimates Navigator. This tool will guide you step by step through the process of creating your country's HIV Estimates.  
+At each step of the way you will be presented with a task to complete. We ask that you read the instructions carefully and use the extra resources and links provided if necessary to complete the task. 
+When you believe you have completed the task, toggle the task complete/incomplete button in the bottom right by clicking on it, and then click "What's next" to see your next task.  </v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -2255,15 +2275,16 @@
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
     </row>
-    <row r="6" spans="1:30" ht="215.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>183</v>
+      <c r="C6" s="61" t="str">
+        <f t="shared" ref="C6:C10" si="0">_xlfn.CONCAT("FRENCH ", B6)</f>
+        <v>FRENCH Are you ready to begin the estimates process?</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>27</v>
@@ -2271,8 +2292,13 @@
       <c r="E6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>183</v>
+      <c r="F6" s="15" t="str">
+        <f t="shared" ref="F6:F10" si="1">_xlfn.CONCAT("FRENCH ", E6)</f>
+        <v>FRENCH In order to proceed to use the Navigator your country must have: 
+ - Collected data from all sites for the time period used in the models;
+ - Compiled and validated the data;
+ - Authorized you to prepare the estimates on behalf of the country. 
+If you are satisfied that the above requirements are met, mark this task and complete and click "What's next?"</v>
       </c>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
@@ -2301,22 +2327,24 @@
       <c r="AC6" s="4"/>
       <c r="AD6" s="4"/>
     </row>
-    <row r="7" spans="1:30" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>183</v>
+      <c r="C7" s="61" t="str">
+        <f t="shared" si="0"/>
+        <v>FRENCH Milestone: Preparing Input Data for HIV Estimates</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="21"/>
-      <c r="F7" s="15" t="s">
-        <v>183</v>
+      <c r="F7" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">FRENCH </v>
       </c>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
@@ -2343,22 +2371,24 @@
       <c r="AC7" s="4"/>
       <c r="AD7" s="4"/>
     </row>
-    <row r="8" spans="1:30" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>183</v>
+      <c r="C8" s="61" t="str">
+        <f t="shared" si="0"/>
+        <v>FRENCH Milestone: Upload Estimates Inputs Data to ADR</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="19"/>
-      <c r="F8" s="15" t="s">
-        <v>183</v>
+      <c r="F8" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">FRENCH </v>
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
@@ -2385,22 +2415,24 @@
       <c r="AC8" s="4"/>
       <c r="AD8" s="4"/>
     </row>
-    <row r="9" spans="1:30" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>183</v>
+      <c r="C9" s="61" t="str">
+        <f t="shared" si="0"/>
+        <v>FRENCH Milestone: Review quality of programme data inputs in ShinyRob</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>38</v>
       </c>
       <c r="E9" s="19"/>
-      <c r="F9" s="15" t="s">
-        <v>183</v>
+      <c r="F9" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">FRENCH </v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
@@ -2427,22 +2459,24 @@
       <c r="AC9" s="4"/>
       <c r="AD9" s="4"/>
     </row>
-    <row r="10" spans="1:30" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>183</v>
+      <c r="C10" s="61" t="str">
+        <f t="shared" si="0"/>
+        <v>FRENCH Milestone: Enter Data Into Spectrum</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>41</v>
       </c>
       <c r="E10" s="19"/>
-      <c r="F10" s="15" t="s">
-        <v>183</v>
+      <c r="F10" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">FRENCH </v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -30986,7 +31020,7 @@
     <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -30994,9 +31028,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O996"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -31018,22 +31052,22 @@
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57" t="s">
-        <v>184</v>
-      </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="56" t="s">
+      <c r="B1" s="55" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="56"/>
+      <c r="D1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="56"/>
+      <c r="E1" s="54"/>
       <c r="F1" s="59" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G1" s="60"/>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="54"/>
+      <c r="I1" s="52"/>
       <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
@@ -31044,22 +31078,22 @@
       <c r="A2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="52" t="s">
-        <v>183</v>
-      </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="55" t="s">
+      <c r="B2" s="57" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="58"/>
+      <c r="D2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="52" t="s">
-        <v>183</v>
-      </c>
-      <c r="G2" s="53"/>
-      <c r="H2" s="55" t="s">
+      <c r="E2" s="53"/>
+      <c r="F2" s="57" t="s">
+        <v>180</v>
+      </c>
+      <c r="G2" s="58"/>
+      <c r="H2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="55"/>
+      <c r="I2" s="53"/>
       <c r="J2" s="5">
         <v>0.1</v>
       </c>
@@ -31084,25 +31118,25 @@
         <v>10</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>14</v>
@@ -31131,25 +31165,25 @@
         <v>44</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>46</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H5" s="30" t="s">
         <v>47</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="J5" s="31"/>
       <c r="K5" s="18">
@@ -31172,25 +31206,25 @@
         <v>50</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>52</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H6" s="30" t="s">
         <v>53</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="J6" s="32"/>
       <c r="K6" s="20">
@@ -31213,25 +31247,25 @@
         <v>56</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>57</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H7" s="17" t="s">
         <v>59</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="J7" s="31"/>
       <c r="K7" s="18">
@@ -31256,19 +31290,19 @@
         <v>63</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>64</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>65</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>66</v>
@@ -31295,19 +31329,19 @@
         <v>69</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>70</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>71</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
@@ -31336,19 +31370,19 @@
         <v>75</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>76</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>77</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
@@ -31375,19 +31409,19 @@
         <v>81</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>82</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>83</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
@@ -31414,19 +31448,19 @@
         <v>88</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>89</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>90</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
@@ -32700,8 +32734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="F7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -32722,10 +32756,10 @@
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="54"/>
+      <c r="C1" s="52"/>
       <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
@@ -32738,10 +32772,10 @@
       <c r="A2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="55"/>
+      <c r="C2" s="53"/>
       <c r="D2" s="6" t="s">
         <v>94</v>
       </c>
@@ -33005,10 +33039,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="54"/>
+      <c r="C1" s="52"/>
       <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
@@ -33021,14 +33055,14 @@
       <c r="A2" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="55"/>
+      <c r="E2" s="53"/>
       <c r="F2" s="5">
         <v>0.1</v>
       </c>
@@ -34322,8 +34356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -34345,10 +34379,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="54"/>
+      <c r="C1" s="52"/>
       <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
@@ -34361,14 +34395,14 @@
       <c r="A2" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="55"/>
+      <c r="E2" s="53"/>
       <c r="F2" s="5">
         <v>0.1</v>
       </c>

</xml_diff>

<commit_message>
NAV-254 update test data file to use pt_PT language id for Portuguese
</commit_message>
<xml_diff>
--- a/navigator_engine/tests/test_data/Estimates Test Data.xlsx
+++ b/navigator_engine/tests/test_data/Estimates Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soppe\Documents\Projects\navigator_engine\navigator_engine\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1754BC-FEF2-4AC9-92F0-31DBD39A467B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41ECA24-F9F1-48BD-AF80-052AA325D989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="192">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -146,9 +146,6 @@
     <t>Country has collected data from all sites for the time period used in the models
 Data are compiled and validated by country (e.g., MOH) authorities.
 The user is authorized to prepare estimates on behalf of the country</t>
-  </si>
-  <si>
-    <t>Congratulations, you have completed this year's estimates process. You may now use your results for other needs such as the PEPFAR data pack, DMPPT2 (for VMMC data where applicable), national reporting, or other needs.</t>
   </si>
   <si>
     <t>Ref.</t>
@@ -1222,52 +1219,49 @@
     <t>check_manual_confirmation('EST-GEN-07-01-A')</t>
   </si>
   <si>
-    <r>
-      <t>In this milestone, you will prepare</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">and place the required input data in the templates needed to generate HIV estimates. You should use the best, highest quality, and most complete input data you have available to you for the estimates process. </t>
-    </r>
+    <t>Milestone Title (Visible to User):::fr</t>
   </si>
   <si>
-    <t>FR::Complete Message</t>
+    <t>Milestone Title (Visible to User):::pt_PT</t>
   </si>
   <si>
-    <t>FRENCH</t>
+    <t>Milestone Description (Visible to User):::fr</t>
   </si>
   <si>
-    <t>Milestone Title (Visible to User):::FR</t>
+    <t>Complete Message::fr</t>
   </si>
   <si>
-    <t>Milestone Description (Visible to User):::FR</t>
+    <t>Milestone Description (Visible to User):::pt_PT</t>
   </si>
   <si>
-    <t>Task Title (Visible to User)::FR</t>
+    <t>Complete Message::pt_PT</t>
   </si>
   <si>
-    <t>If test fails, present this to user:::FR</t>
+    <t>Task Title (Visible to User)::fr</t>
   </si>
   <si>
-    <t>Resources / Links::FR</t>
+    <t>Task Title (Visible to User)::pt_PT</t>
   </si>
   <si>
-    <t>Task Test (if test passes, proceed to next test)::FR</t>
+    <t>If test fails, present this to user:::fr</t>
+  </si>
+  <si>
+    <t>If test fails, present this to user:::pt_PT</t>
+  </si>
+  <si>
+    <t>Resources / Links::fr</t>
+  </si>
+  <si>
+    <t>Resources / Links::pt_PT</t>
+  </si>
+  <si>
+    <t>Test Milestone</t>
+  </si>
+  <si>
+    <t>Test Complete Message</t>
+  </si>
+  <si>
+    <t>Test Resource 1, Test resource 2, Test link https://test.org</t>
   </si>
 </sst>
 </file>
@@ -1500,7 +1494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1608,30 +1602,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2020,11 +1998,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD993"/>
+  <dimension ref="A1:AG993"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2040,40 +2018,48 @@
     <col min="11" max="11" width="17.44140625" customWidth="1"/>
     <col min="12" max="12" width="28.88671875" customWidth="1"/>
     <col min="13" max="13" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="27" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="27" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52" t="s">
+      <c r="I1" s="52"/>
+      <c r="J1" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="52"/>
+      <c r="L1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="52"/>
-      <c r="I1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="51" t="s">
-        <v>179</v>
-      </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
@@ -2088,41 +2074,54 @@
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
-    </row>
-    <row r="2" spans="1:30" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4"/>
+    </row>
+    <row r="2" spans="1:33" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="61" t="str">
-        <f>_xlfn.CONCAT("FRENCH ", A2)</f>
+      <c r="B2" s="55" t="str">
+        <f>_xlfn.CONCAT("FRENCH ", $A2)</f>
         <v>FRENCH Test Data Overview</v>
       </c>
-      <c r="C2" s="62" t="s">
-        <v>178</v>
-      </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53" t="str">
-        <f>_xlfn.CONCAT("FRENCH ", C2)</f>
-        <v xml:space="preserve">FRENCH In this milestone, you will prepare and place the required input data in the templates needed to generate HIV estimates. You should use the best, highest quality, and most complete input data you have available to you for the estimates process. </v>
-      </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53" t="s">
+      <c r="C2" s="55" t="str">
+        <f>_xlfn.CONCAT("PORTUGUESE ",$A2)</f>
+        <v>PORTUGUESE Test Data Overview</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53" t="str">
+        <f>_xlfn.CONCAT("FRENCH ", D2)</f>
+        <v>FRENCH Test Milestone</v>
+      </c>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53" t="str">
+        <f>_xlfn.CONCAT("PORTUGUESE ", D2)</f>
+        <v>PORTUGUESE Test Milestone</v>
+      </c>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="5">
+      <c r="K2" s="53"/>
+      <c r="L2" s="5">
         <v>0.1</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="5" t="str">
-        <f>_xlfn.CONCAT("FRENCH ", J2)</f>
-        <v>FRENCH Congratulations, you have completed this year's estimates process. You may now use your results for other needs such as the PEPFAR data pack, DMPPT2 (for VMMC data where applicable), national reporting, or other needs.</v>
-      </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="M2" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="N2" s="51" t="str">
+        <f>_xlfn.CONCAT("FRENCH ", M2)</f>
+        <v>FRENCH Test Complete Message</v>
+      </c>
+      <c r="O2" s="51" t="str">
+        <f>_xlfn.CONCAT("PORTUGUESE ", M2)</f>
+        <v>PORTUGUESE Test Complete Message</v>
+      </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
@@ -2137,8 +2136,11 @@
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
       <c r="AD2" s="4"/>
-    </row>
-    <row r="3" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+    </row>
+    <row r="3" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -2167,52 +2169,58 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
     </row>
-    <row r="4" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>10</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>183</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="G4" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="J4" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="L4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="I4" s="11" t="s">
+      <c r="M4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="N4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="O4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="R4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="O4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
@@ -2224,45 +2232,64 @@
       <c r="AB4" s="4"/>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
-    </row>
-    <row r="5" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+    </row>
+    <row r="5" spans="1:33" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="61" t="str">
+      <c r="C5" s="55" t="str">
         <f>_xlfn.CONCAT("FRENCH ", B5)</f>
         <v>FRENCH Welcome to the Navigator</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="55" t="str">
+        <f>_xlfn.CONCAT("PORTUGUESE ",$B5)</f>
+        <v>PORTUGUESE Welcome to the Navigator</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="15" t="str">
-        <f>_xlfn.CONCAT("FRENCH ", E5)</f>
+      <c r="G5" s="15" t="str">
+        <f>_xlfn.CONCAT("FRENCH ", $F5)</f>
         <v xml:space="preserve">FRENCH Welcome to the HIV Estimates Navigator. This tool will guide you step by step through the process of creating your country's HIV Estimates.  
 At each step of the way you will be presented with a task to complete. We ask that you read the instructions carefully and use the extra resources and links provided if necessary to complete the task. 
 When you believe you have completed the task, toggle the task complete/incomplete button in the bottom right by clicking on it, and then click "What's next" to see your next task.  </v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16">
+      <c r="H5" s="15" t="str">
+        <f>_xlfn.CONCAT("PORTUGUESE ",$F5)</f>
+        <v xml:space="preserve">PORTUGUESE Welcome to the HIV Estimates Navigator. This tool will guide you step by step through the process of creating your country's HIV Estimates.  
+At each step of the way you will be presented with a task to complete. We ask that you read the instructions carefully and use the extra resources and links provided if necessary to complete the task. 
+When you believe you have completed the task, toggle the task complete/incomplete button in the bottom right by clicking on it, and then click "What's next" to see your next task.  </v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="J5" s="15" t="str">
+        <f>_xlfn.CONCAT("FRENCH ", $I5)</f>
+        <v>FRENCH Test Resource 1, Test resource 2, Test link https://test.org</v>
+      </c>
+      <c r="K5" s="15" t="str">
+        <f>_xlfn.CONCAT("PORTUGUESE ",$I5)</f>
+        <v>PORTUGUESE Test Resource 1, Test resource 2, Test link https://test.org</v>
+      </c>
+      <c r="L5" s="16">
         <v>1</v>
       </c>
-      <c r="J5" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="O5" s="18"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
+      <c r="M5" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="R5" s="18"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
@@ -2274,47 +2301,60 @@
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
-    </row>
-    <row r="6" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="4"/>
+    </row>
+    <row r="6" spans="1:33" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="61" t="str">
+      <c r="C6" s="55" t="str">
         <f t="shared" ref="C6:C10" si="0">_xlfn.CONCAT("FRENCH ", B6)</f>
         <v>FRENCH Are you ready to begin the estimates process?</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="55" t="str">
+        <f t="shared" ref="D6:D10" si="1">_xlfn.CONCAT("PORTUGUESE ",$B6)</f>
+        <v>PORTUGUESE Are you ready to begin the estimates process?</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="15" t="str">
-        <f t="shared" ref="F6:F10" si="1">_xlfn.CONCAT("FRENCH ", E6)</f>
+      <c r="G6" s="15" t="str">
+        <f>_xlfn.CONCAT("FRENCH ", $F6)</f>
         <v>FRENCH In order to proceed to use the Navigator your country must have: 
  - Collected data from all sites for the time period used in the models;
  - Compiled and validated the data;
  - Authorized you to prepare the estimates on behalf of the country. 
 If you are satisfied that the above requirements are met, mark this task and complete and click "What's next?"</v>
       </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="16">
+      <c r="H6" s="15" t="str">
+        <f>_xlfn.CONCAT("PORTUGUESE ",$F6)</f>
+        <v>PORTUGUESE In order to proceed to use the Navigator your country must have: 
+ - Collected data from all sites for the time period used in the models;
+ - Compiled and validated the data;
+ - Authorized you to prepare the estimates on behalf of the country. 
+If you are satisfied that the above requirements are met, mark this task and complete and click "What's next?"</v>
+      </c>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="16">
         <v>1</v>
       </c>
-      <c r="J6" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="O6" s="20"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
+      <c r="M6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="R6" s="20"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
@@ -2326,39 +2366,42 @@
       <c r="AB6" s="4"/>
       <c r="AC6" s="4"/>
       <c r="AD6" s="4"/>
-    </row>
-    <row r="7" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="4"/>
+    </row>
+    <row r="7" spans="1:33" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="61" t="str">
+      <c r="C7" s="55" t="str">
         <f t="shared" si="0"/>
         <v>FRENCH Milestone: Preparing Input Data for HIV Estimates</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="15" t="str">
+      <c r="D7" s="55" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">FRENCH </v>
-      </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="16">
+        <v>PORTUGUESE Milestone: Preparing Input Data for HIV Estimates</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="16">
         <v>1</v>
       </c>
-      <c r="J7" s="22"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="O7" s="18"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="R7" s="18"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
@@ -2370,39 +2413,42 @@
       <c r="AB7" s="4"/>
       <c r="AC7" s="4"/>
       <c r="AD7" s="4"/>
-    </row>
-    <row r="8" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="4"/>
+    </row>
+    <row r="8" spans="1:33" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="61" t="str">
+      <c r="C8" s="55" t="str">
         <f t="shared" si="0"/>
         <v>FRENCH Milestone: Upload Estimates Inputs Data to ADR</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="15" t="str">
+      <c r="D8" s="55" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">FRENCH </v>
-      </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="16">
+        <v>PORTUGUESE Milestone: Upload Estimates Inputs Data to ADR</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="16">
         <v>1</v>
       </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="O8" s="18"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="R8" s="18"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
@@ -2414,39 +2460,42 @@
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
       <c r="AD8" s="4"/>
-    </row>
-    <row r="9" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="4"/>
+    </row>
+    <row r="9" spans="1:33" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="61" t="str">
+      <c r="C9" s="55" t="str">
         <f t="shared" si="0"/>
         <v>FRENCH Milestone: Review quality of programme data inputs in ShinyRob</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="15" t="str">
+      <c r="D9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">FRENCH </v>
-      </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="16">
+        <v>PORTUGUESE Milestone: Review quality of programme data inputs in ShinyRob</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="16">
         <v>0</v>
       </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="O9" s="18"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="R9" s="18"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
@@ -2458,39 +2507,42 @@
       <c r="AB9" s="4"/>
       <c r="AC9" s="4"/>
       <c r="AD9" s="4"/>
-    </row>
-    <row r="10" spans="1:30" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="4"/>
+    </row>
+    <row r="10" spans="1:33" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="61" t="str">
+      <c r="C10" s="55" t="str">
         <f t="shared" si="0"/>
         <v>FRENCH Milestone: Enter Data Into Spectrum</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="15" t="str">
+      <c r="D10" s="55" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">FRENCH </v>
-      </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="16">
+        <v>PORTUGUESE Milestone: Enter Data Into Spectrum</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="16">
         <v>1</v>
       </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="O10" s="18"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="R10" s="18"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
@@ -2502,8 +2554,11 @@
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
       <c r="AD10" s="4"/>
-    </row>
-    <row r="11" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="4"/>
+    </row>
+    <row r="11" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2532,7 +2587,7 @@
       <c r="Z11" s="4"/>
       <c r="AA11" s="4"/>
     </row>
-    <row r="12" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2561,7 +2616,7 @@
       <c r="Z12" s="4"/>
       <c r="AA12" s="4"/>
     </row>
-    <row r="13" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2590,7 +2645,7 @@
       <c r="Z13" s="4"/>
       <c r="AA13" s="4"/>
     </row>
-    <row r="14" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2619,7 +2674,7 @@
       <c r="Z14" s="4"/>
       <c r="AA14" s="4"/>
     </row>
-    <row r="15" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2648,7 +2703,7 @@
       <c r="Z15" s="4"/>
       <c r="AA15" s="4"/>
     </row>
-    <row r="16" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -31011,13 +31066,15 @@
       <c r="AA993" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
+  <mergeCells count="8">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -31026,11 +31083,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O996"/>
+  <dimension ref="A1:K996"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -31048,59 +31105,43 @@
     <col min="12" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55" t="s">
-        <v>181</v>
-      </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="54" t="s">
+      <c r="B1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="G1" s="60"/>
-      <c r="H1" s="52" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="52"/>
-      <c r="J1" s="2" t="s">
+      <c r="E1" s="52"/>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-    </row>
-    <row r="2" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="58"/>
+        <v>41</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="53"/>
       <c r="D2" s="53" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="53"/>
-      <c r="F2" s="57" t="s">
-        <v>180</v>
-      </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="5">
+      <c r="F2" s="5">
         <v>0.1</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
       <c r="B3" s="26"/>
       <c r="C3" s="7"/>
@@ -31110,382 +31151,284 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="C4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="H4" s="10" t="s">
+      <c r="F4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>185</v>
+      <c r="G4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="J4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="184.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="C5" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>180</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="F5" s="17" t="s">
+      <c r="E5" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="H5" s="30" t="s">
+      <c r="F5" s="31"/>
+      <c r="G5" s="18">
+        <v>0</v>
+      </c>
+      <c r="H5" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="18">
-        <v>0</v>
-      </c>
-      <c r="L5" s="17" t="s">
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="204.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="B6" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="C6" s="17" t="s">
         <v>50</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>180</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="F6" s="17" t="s">
+      <c r="E6" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="H6" s="30" t="s">
+      <c r="F6" s="32"/>
+      <c r="G6" s="20">
+        <v>1</v>
+      </c>
+      <c r="H6" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="I6" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="J6" s="32"/>
-      <c r="K6" s="20">
-        <v>1</v>
-      </c>
-      <c r="L6" s="17" t="s">
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="214.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="B7" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="C7" s="17" t="s">
         <v>56</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>180</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="F7" s="17" t="s">
+      <c r="E7" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="H7" s="17" t="s">
+      <c r="F7" s="31"/>
+      <c r="G7" s="18">
+        <v>1</v>
+      </c>
+      <c r="H7" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="18">
-        <v>1</v>
-      </c>
-      <c r="L7" s="33" t="s">
+      <c r="I7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="M7" s="23" t="s">
+      <c r="J7" s="17"/>
+      <c r="K7" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="204.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="B8" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="C8" s="17" t="s">
         <v>63</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>180</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="F8" s="17" t="s">
+      <c r="E8" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G8" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="H8" s="17" t="s">
+      <c r="F8" s="31"/>
+      <c r="G8" s="18">
+        <v>1</v>
+      </c>
+      <c r="H8" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="18">
-        <v>1</v>
-      </c>
-      <c r="L8" s="23" t="s">
+      <c r="I8" s="23"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="286.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="M8" s="23"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="B9" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="C9" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>180</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="31">
+        <v>1</v>
+      </c>
+      <c r="G9" s="18">
+        <v>1</v>
+      </c>
+      <c r="H9" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="31">
-        <v>1</v>
-      </c>
-      <c r="K9" s="18">
-        <v>1</v>
-      </c>
-      <c r="L9" s="23" t="s">
+      <c r="I9" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="M9" s="23" t="s">
+      <c r="J9" s="17"/>
+      <c r="K9" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="61.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="163.80000000000001" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="B10" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="C10" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>180</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="F10" s="17" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="18">
+        <v>0</v>
+      </c>
+      <c r="H10" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="18">
-        <v>0</v>
-      </c>
-      <c r="L10" s="23" t="s">
+      <c r="I10" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="M10" s="23" t="s">
+      <c r="J10" s="17"/>
+      <c r="K10" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="163.80000000000001" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="B11" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="C11" s="17" t="s">
         <v>81</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>180</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="F11" s="17" t="s">
+      <c r="E11" s="17"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="18">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="18">
-        <v>0</v>
-      </c>
-      <c r="L11" s="5" t="s">
+      <c r="I11" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="M11" s="34" t="s">
+      <c r="J11" s="17"/>
+      <c r="K11" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17" t="s">
+    </row>
+    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="B12" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="C12" s="17" t="s">
         <v>88</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>180</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="F12" s="17" t="s">
+      <c r="E12" s="17"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="35">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="35">
-        <v>0</v>
-      </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="36"/>
       <c r="H13" s="24"/>
     </row>
-    <row r="14" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H14" s="24"/>
     </row>
-    <row r="15" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H16" s="24"/>
     </row>
     <row r="17" spans="8:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -32711,19 +32654,15 @@
     <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H5" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="H6" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -32735,7 +32674,7 @@
   <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -32770,14 +32709,14 @@
     </row>
     <row r="2" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="53" t="s">
         <v>92</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>93</v>
       </c>
       <c r="C2" s="53"/>
       <c r="D2" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" s="39"/>
       <c r="F2" s="5">
@@ -32796,54 +32735,54 @@
     </row>
     <row r="4" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="G4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="72" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="C5" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="D5" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="30" t="s">
         <v>98</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>99</v>
       </c>
       <c r="F5" s="43">
         <v>1</v>
@@ -32852,26 +32791,26 @@
         <v>0</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
       <c r="K5" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="C6" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="17" t="s">
         <v>104</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>105</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="43">
@@ -32881,29 +32820,29 @@
         <v>0</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I6" s="23"/>
       <c r="J6" s="17"/>
       <c r="K6" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="82.2" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="C7" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>110</v>
-      </c>
       <c r="D7" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="43">
         <v>0</v>
@@ -32912,28 +32851,28 @@
         <v>0</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I7" s="17"/>
       <c r="J7" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="K7" s="15" t="s">
         <v>112</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="102.6" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="C8" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="D8" s="17" t="s">
         <v>116</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>117</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="43">
@@ -32943,14 +32882,14 @@
         <v>0</v>
       </c>
       <c r="H8" s="44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M8" s="45"/>
       <c r="N8" s="45"/>
@@ -32969,19 +32908,19 @@
     </row>
     <row r="9" spans="1:26" ht="72" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="C9" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>123</v>
-      </c>
       <c r="E9" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" s="17">
         <v>0</v>
@@ -32993,7 +32932,7 @@
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
       <c r="K9" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -33053,14 +32992,14 @@
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="53" t="s">
         <v>125</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>126</v>
       </c>
       <c r="C2" s="53"/>
       <c r="D2" s="53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E2" s="53"/>
       <c r="F2" s="5">
@@ -33079,51 +33018,51 @@
     </row>
     <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="G4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="102.6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="C5" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="D5" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>131</v>
-      </c>
       <c r="E5" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="31">
         <v>1</v>
@@ -33132,28 +33071,28 @@
         <v>0</v>
       </c>
       <c r="H5" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="82.2" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="C6" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="E6" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>138</v>
       </c>
       <c r="F6" s="31">
         <v>1</v>
@@ -33163,19 +33102,19 @@
       </c>
       <c r="H6" s="32"/>
       <c r="I6" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B7" s="46"/>
       <c r="C7" s="46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D7" s="46"/>
       <c r="E7" s="46"/>
@@ -33186,30 +33125,30 @@
         <v>1</v>
       </c>
       <c r="H7" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="I7" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>143</v>
-      </c>
       <c r="J7" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="C8" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="D8" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="E8" s="17" t="s">
         <v>147</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>148</v>
       </c>
       <c r="F8" s="31">
         <v>1</v>
@@ -33220,24 +33159,24 @@
       <c r="H8" s="32"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="C9" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>153</v>
-      </c>
       <c r="E9" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F9" s="32">
         <v>1</v>
@@ -33248,21 +33187,21 @@
       <c r="H9" s="32"/>
       <c r="I9" s="22"/>
       <c r="J9" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="154.19999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="C10" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="D10" s="17" t="s">
         <v>157</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>158</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="31">
@@ -33274,7 +33213,7 @@
       <c r="H10" s="17"/>
       <c r="I10" s="49"/>
       <c r="J10" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -34393,14 +34332,14 @@
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="53"/>
       <c r="D2" s="53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E2" s="53"/>
       <c r="F2" s="5">
@@ -34419,51 +34358,51 @@
     </row>
     <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="G4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="102.6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B5" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="D5" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>131</v>
-      </c>
       <c r="E5" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="31">
         <v>1</v>
@@ -34472,28 +34411,28 @@
         <v>0</v>
       </c>
       <c r="H5" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="82.2" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="E6" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>138</v>
       </c>
       <c r="F6" s="31">
         <v>1</v>
@@ -34504,16 +34443,16 @@
       <c r="H6" s="32"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B7" s="46"/>
       <c r="C7" s="46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D7" s="46"/>
       <c r="E7" s="46"/>
@@ -34524,30 +34463,30 @@
         <v>1</v>
       </c>
       <c r="H7" s="48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I7" s="50" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="D8" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="E8" s="17" t="s">
         <v>147</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>148</v>
       </c>
       <c r="F8" s="31">
         <v>1</v>
@@ -34557,27 +34496,27 @@
       </c>
       <c r="H8" s="32"/>
       <c r="I8" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>153</v>
-      </c>
       <c r="E9" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F9" s="32">
         <v>1</v>
@@ -34588,21 +34527,21 @@
       <c r="H9" s="32"/>
       <c r="I9" s="22"/>
       <c r="J9" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="154.19999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B10" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="D10" s="17" t="s">
         <v>157</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>158</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="31">
@@ -34614,7 +34553,7 @@
       <c r="H10" s="17"/>
       <c r="I10" s="49"/>
       <c r="J10" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>